<commit_message>
ooSQLite - make some arguments optional; othewise chages are formatting changes
git-svn-id: file:///local/rexx/oorexx/oorexx.svn@7929 0b6cbdbe-3aab-466e-b73a-abd511dda0a2
</commit_message>
<xml_diff>
--- a/incubator/ooSQLite/doc/StatusAllSQLiteFunctions.xlsx
+++ b/incubator/ooSQLite/doc/StatusAllSQLiteFunctions.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="30" windowWidth="18195" windowHeight="11310"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="244">
   <si>
     <t>sqlite3_aggregate_context</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>sqlite3_backup_finish</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> need to implement ooSQLiteBackup class</t>
   </si>
   <si>
     <t>sqlite3_backup_init</t>
@@ -1214,8 +1211,8 @@
   <dimension ref="A1:C207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <pane ySplit="4" topLeftCell="A185" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,20 +1224,20 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1248,10 +1245,10 @@
         <v>0</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1259,7 +1256,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -1270,10 +1267,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1281,736 +1278,728 @@
         <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="12" t="s">
         <v>20</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="12" t="s">
-        <v>23</v>
-      </c>
       <c r="C23" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C24" s="5"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C40" s="12"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C43" s="12"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C45" s="12"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C50" s="12"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C52" s="12"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C54" s="12"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C56" s="12"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C63" s="12"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C66" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C67" s="12"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C69" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C70" s="12"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C72" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C73" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C82" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B87" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C87" s="12"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C89" t="s">
         <v>2</v>
@@ -2018,97 +2007,97 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C92" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C94" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C95" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C98" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C99" t="s">
         <v>2</v>
@@ -2116,94 +2105,94 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C100" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B106" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B107" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C107" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C108" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C109" t="s">
         <v>2</v>
@@ -2211,532 +2200,532 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C112" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C113" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C114" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C115" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C116" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C117" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C118" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C119" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C120" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B121" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="C121" t="s">
         <v>215</v>
-      </c>
-      <c r="C121" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B122" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C122" s="12"/>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C123" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C124" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C125" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B126" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C126" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B127" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="C127" t="s">
         <v>215</v>
-      </c>
-      <c r="C127" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B128" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="C128" t="s">
         <v>215</v>
-      </c>
-      <c r="C128" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B129" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C129" s="12"/>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C130" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C131" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B134" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C134" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B137" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C138" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C139" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C140" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B141" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C141" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B142" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C142" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C143" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C144" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B145" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C145" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B146" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C146" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B147" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C147" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B148" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C148" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B149" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C149" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B150" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C150" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B151" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C151" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C152" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B153" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C153" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B156" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C156" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B157" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C157" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B158" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C158" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B159" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C159" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B160" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C160" t="s">
         <v>2</v>
@@ -2744,115 +2733,115 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B169" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C169" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B170" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C170" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B172" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C172" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B173" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C173" t="s">
         <v>2</v>
@@ -2860,37 +2849,37 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B174" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B175" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B176" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C176" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B177" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C177" t="s">
         <v>2</v>
@@ -2898,314 +2887,314 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B178" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C178" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B179" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B180" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C180" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B181" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C181" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B182" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C182" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B183" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C183" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C184" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C185" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B186" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C186" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B187" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C187" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B188" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C188" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B189" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C189" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B190" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C190" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C191" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B192" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C192" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B193" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C193" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B194" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C194" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B195" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C195" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B196" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B197" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C197" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B198" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C198" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B199" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C199" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B200" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C200" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B201" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C201" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B202" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C202" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B203" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C203" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update implementation table in ooSQLite doc directory
git-svn-id: file:///local/rexx/oorexx/oorexx.svn@7962 0b6cbdbe-3aab-466e-b73a-abd511dda0a2
</commit_message>
<xml_diff>
--- a/incubator/ooSQLite/doc/StatusAllSQLiteFunctions.xlsx
+++ b/incubator/ooSQLite/doc/StatusAllSQLiteFunctions.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="245">
   <si>
     <t>sqlite3_aggregate_context</t>
   </si>
@@ -713,9 +713,6 @@
     <t>As oosqlPrepare() and .ooSQLiteStmt~new()</t>
   </si>
   <si>
-    <t>Used by implementation code</t>
-  </si>
-  <si>
     <t>Rexx has its own sleep</t>
   </si>
   <si>
@@ -765,6 +762,12 @@
   </si>
   <si>
     <t>used when creating new SQL functions and aggregates</t>
+  </si>
+  <si>
+    <t>Implemented indirectly in the equote() method and ooSQLiteEnquote()</t>
+  </si>
+  <si>
+    <t>Implemented indirectly, used by implementation code</t>
   </si>
 </sst>
 </file>
@@ -1211,15 +1214,15 @@
   <dimension ref="A1:C207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A185" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9:C12"/>
+      <pane ySplit="4" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47" customWidth="1"/>
-    <col min="3" max="3" width="62.28515625" customWidth="1"/>
+    <col min="3" max="3" width="66.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1282,7 +1285,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1291,7 +1294,7 @@
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1300,7 +1303,7 @@
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -1309,7 +1312,7 @@
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -1531,7 +1534,7 @@
         <v>217</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1769,7 +1772,7 @@
         <v>217</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1780,7 +1783,7 @@
         <v>217</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1791,7 +1794,7 @@
         <v>214</v>
       </c>
       <c r="C66" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1811,7 +1814,7 @@
         <v>217</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1822,7 +1825,7 @@
         <v>214</v>
       </c>
       <c r="C69" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -1853,7 +1856,7 @@
         <v>214</v>
       </c>
       <c r="C72" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -1864,7 +1867,7 @@
         <v>220</v>
       </c>
       <c r="C73" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -1939,7 +1942,7 @@
         <v>220</v>
       </c>
       <c r="C82" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -1950,7 +1953,7 @@
         <v>220</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -2029,7 +2032,7 @@
         <v>220</v>
       </c>
       <c r="C92" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -2041,14 +2044,14 @@
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="7" t="s">
+      <c r="A94" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B94" s="7" t="s">
-        <v>214</v>
+      <c r="B94" t="s">
+        <v>10</v>
       </c>
       <c r="C94" t="s">
-        <v>216</v>
+        <v>244</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -2078,7 +2081,7 @@
         <v>217</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -2104,14 +2107,14 @@
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="7" t="s">
+      <c r="A100" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B100" s="7" t="s">
-        <v>214</v>
+      <c r="B100" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="C100" t="s">
-        <v>226</v>
+        <v>244</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -2162,7 +2165,7 @@
         <v>220</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -2177,14 +2180,14 @@
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="7" t="s">
+      <c r="A108" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B108" s="7" t="s">
-        <v>214</v>
+      <c r="B108" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="C108" t="s">
-        <v>216</v>
+        <v>244</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -2215,11 +2218,11 @@
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="7" t="s">
+      <c r="A112" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B112" s="7" t="s">
-        <v>214</v>
+      <c r="B112" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="C112" t="s">
         <v>216</v>
@@ -2233,7 +2236,7 @@
         <v>10</v>
       </c>
       <c r="C113" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -2244,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="C114" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -2255,7 +2258,7 @@
         <v>10</v>
       </c>
       <c r="C115" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -2277,7 +2280,7 @@
         <v>10</v>
       </c>
       <c r="C117" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -2299,7 +2302,7 @@
         <v>10</v>
       </c>
       <c r="C119" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -2310,7 +2313,7 @@
         <v>10</v>
       </c>
       <c r="C120" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -2374,7 +2377,7 @@
         <v>220</v>
       </c>
       <c r="C126" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -2427,7 +2430,7 @@
         <v>10</v>
       </c>
       <c r="C131" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -2447,14 +2450,14 @@
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" s="7" t="s">
+      <c r="A134" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B134" s="7" t="s">
-        <v>214</v>
+      <c r="B134" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="C134" t="s">
-        <v>216</v>
+        <v>244</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -2481,7 +2484,7 @@
         <v>220</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -2688,14 +2691,14 @@
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A157" s="7" t="s">
+      <c r="A157" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="B157" s="7" t="s">
-        <v>214</v>
+      <c r="B157" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="C157" t="s">
-        <v>226</v>
+        <v>244</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -2706,18 +2709,18 @@
         <v>220</v>
       </c>
       <c r="C158" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A159" s="7" t="s">
+      <c r="A159" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B159" s="7" t="s">
-        <v>214</v>
+      <c r="B159" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="C159" t="s">
-        <v>216</v>
+        <v>243</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -2871,7 +2874,7 @@
         <v>10</v>
       </c>
       <c r="C176" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -2893,7 +2896,7 @@
         <v>220</v>
       </c>
       <c r="C178" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -2912,7 +2915,7 @@
         <v>220</v>
       </c>
       <c r="C180" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -2923,7 +2926,7 @@
         <v>220</v>
       </c>
       <c r="C181" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -2934,7 +2937,7 @@
         <v>220</v>
       </c>
       <c r="C182" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -3096,7 +3099,7 @@
         <v>220</v>
       </c>
       <c r="C197" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -3107,7 +3110,7 @@
         <v>220</v>
       </c>
       <c r="C198" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
@@ -3118,29 +3121,29 @@
         <v>220</v>
       </c>
       <c r="C199" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A200" s="7" t="s">
+      <c r="A200" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="B200" s="7" t="s">
-        <v>214</v>
+      <c r="B200" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="C200" t="s">
-        <v>216</v>
+        <v>243</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A201" s="7" t="s">
+      <c r="A201" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="B201" s="7" t="s">
-        <v>214</v>
+      <c r="B201" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="C201" t="s">
-        <v>216</v>
+        <v>243</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
@@ -3151,7 +3154,7 @@
         <v>220</v>
       </c>
       <c r="C202" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
@@ -3162,7 +3165,7 @@
         <v>220</v>
       </c>
       <c r="C203" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
ooSQLite - update the implemented SQLite functions list, example clean up
git-svn-id: file:///local/rexx/oorexx/oorexx.svn@9308 0b6cbdbe-3aab-466e-b73a-abd511dda0a2
</commit_message>
<xml_diff>
--- a/incubator/ooSQLite/doc/StatusAllSQLiteFunctions.xlsx
+++ b/incubator/ooSQLite/doc/StatusAllSQLiteFunctions.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="242">
   <si>
     <t>sqlite3_aggregate_context</t>
   </si>
@@ -98,12 +98,6 @@
     <t xml:space="preserve"> no UTF-16 functions implemented</t>
   </si>
   <si>
-    <t>sqlite3_bind_value</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> exists oo and classic as unimplemented</t>
-  </si>
-  <si>
     <t>sqlite3_bind_zeroblob</t>
   </si>
   <si>
@@ -698,9 +692,6 @@
     <t>not planned at this point</t>
   </si>
   <si>
-    <t>used to load static SQLite extension libraries, not understood</t>
-  </si>
-  <si>
     <t>Use of this interface is not recommended</t>
   </si>
   <si>
@@ -725,15 +716,9 @@
     <t>registers callback for tracing</t>
   </si>
   <si>
-    <t>used in loading static SQLite extension libraries, not understood</t>
-  </si>
-  <si>
     <t>will use the xx_v2 functions</t>
   </si>
   <si>
-    <t>used to create custom collations</t>
-  </si>
-  <si>
     <t>virtual tables probably need to be implemented in C/C++</t>
   </si>
   <si>
@@ -746,9 +731,6 @@
     <t>used whe creating new SQL functions and aggregates</t>
   </si>
   <si>
-    <t>used when creating custom collations</t>
-  </si>
-  <si>
     <t>For low-level control of database files, hard to see its use in Rexx</t>
   </si>
   <si>
@@ -768,13 +750,46 @@
   </si>
   <si>
     <t>Implemented indirectly, used by implementation code</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> implemented oo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NEED</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="7" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> classic</t>
+    </r>
+  </si>
+  <si>
+    <t>verb is create collation</t>
+  </si>
+  <si>
+    <t>verb is create function</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -845,8 +860,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -877,6 +900,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -890,7 +919,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -906,6 +935,7 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1214,8 +1244,8 @@
   <dimension ref="A1:C207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B65" sqref="B65"/>
+      <pane ySplit="4" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,20 +1257,20 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1248,10 +1278,10 @@
         <v>0</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>217</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1259,22 +1289,20 @@
         <v>1</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>221</v>
-      </c>
+      <c r="B7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1401,19 +1429,17 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>219</v>
-      </c>
+      <c r="A23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="12"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>10</v>
@@ -1422,73 +1448,73 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>10</v>
@@ -1496,7 +1522,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>10</v>
@@ -1504,7 +1530,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>10</v>
@@ -1512,7 +1538,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>10</v>
@@ -1520,26 +1546,24 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>237</v>
-      </c>
+      <c r="A36" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C36" s="12"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>20</v>
@@ -1547,7 +1571,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>10</v>
@@ -1555,7 +1579,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>10</v>
@@ -1563,7 +1587,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B40" s="12" t="s">
         <v>20</v>
@@ -1572,7 +1596,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>10</v>
@@ -1580,7 +1604,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>10</v>
@@ -1588,7 +1612,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B43" s="12" t="s">
         <v>20</v>
@@ -1597,7 +1621,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>10</v>
@@ -1605,7 +1629,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B45" s="12" t="s">
         <v>20</v>
@@ -1614,7 +1638,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>10</v>
@@ -1622,7 +1646,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>10</v>
@@ -1630,7 +1654,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>10</v>
@@ -1638,7 +1662,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>10</v>
@@ -1646,7 +1670,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B50" s="12" t="s">
         <v>20</v>
@@ -1655,7 +1679,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>10</v>
@@ -1663,7 +1687,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B52" s="12" t="s">
         <v>20</v>
@@ -1672,7 +1696,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>10</v>
@@ -1680,7 +1704,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B54" s="12" t="s">
         <v>20</v>
@@ -1689,7 +1713,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>10</v>
@@ -1697,7 +1721,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B56" s="12" t="s">
         <v>20</v>
@@ -1706,26 +1730,24 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B58" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C58" s="12" t="s">
-        <v>219</v>
-      </c>
+      <c r="A58" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58" s="12"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>10</v>
@@ -1733,7 +1755,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>10</v>
@@ -1741,7 +1763,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>10</v>
@@ -1749,7 +1771,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>10</v>
@@ -1757,7 +1779,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B63" s="12" t="s">
         <v>20</v>
@@ -1766,40 +1788,40 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C66" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B67" s="12" t="s">
         <v>20</v>
@@ -1807,30 +1829,30 @@
       <c r="C67" s="12"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B68" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="C68" s="12" t="s">
-        <v>232</v>
+      <c r="A68" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C68" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C69" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B70" s="12" t="s">
         <v>20</v>
@@ -1838,41 +1860,41 @@
       <c r="C70" s="12"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B71" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="C71" s="12" t="s">
-        <v>219</v>
+      <c r="A71" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C71" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C72" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C73" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>10</v>
@@ -1880,7 +1902,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>10</v>
@@ -1888,7 +1910,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>10</v>
@@ -1896,7 +1918,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>10</v>
@@ -1904,7 +1926,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>10</v>
@@ -1912,7 +1934,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>10</v>
@@ -1920,7 +1942,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>10</v>
@@ -1928,7 +1950,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>10</v>
@@ -1936,37 +1958,35 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C82" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B83" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>230</v>
-      </c>
+      <c r="A83" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C83" s="1"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>10</v>
@@ -1974,7 +1994,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>10</v>
@@ -1982,7 +2002,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B87" s="12" t="s">
         <v>20</v>
@@ -1991,7 +2011,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B88" s="4" t="s">
         <v>10</v>
@@ -1999,10 +2019,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C89" t="s">
         <v>2</v>
@@ -2010,7 +2030,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>10</v>
@@ -2018,7 +2038,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B91" s="4" t="s">
         <v>10</v>
@@ -2026,18 +2046,18 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C92" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>10</v>
@@ -2045,29 +2065,29 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B94" t="s">
         <v>10</v>
       </c>
       <c r="C94" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C95" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B96" s="4" t="s">
         <v>10</v>
@@ -2075,32 +2095,32 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C98" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C99" t="s">
         <v>2</v>
@@ -2108,18 +2128,18 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B100" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C100" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B101" s="4" t="s">
         <v>10</v>
@@ -2127,7 +2147,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B102" s="4" t="s">
         <v>10</v>
@@ -2135,7 +2155,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B103" s="4" t="s">
         <v>10</v>
@@ -2143,7 +2163,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B104" s="4" t="s">
         <v>10</v>
@@ -2151,51 +2171,49 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C106" s="1"/>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B105" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="B106" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="B107" s="10" t="s">
-        <v>220</v>
+      <c r="B107" s="7" t="s">
+        <v>212</v>
       </c>
       <c r="C107" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B108" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C108" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C109" t="s">
         <v>2</v>
@@ -2203,7 +2221,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B110" s="4" t="s">
         <v>10</v>
@@ -2211,7 +2229,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B111" s="4" t="s">
         <v>10</v>
@@ -2219,117 +2237,117 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B112" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C112" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B113" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C113" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B114" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C114" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B115" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C115" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C116" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B117" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C117" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C118" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B119" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C119" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B120" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C120" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C121" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B122" s="12" t="s">
         <v>20</v>
@@ -2338,73 +2356,73 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B123" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C123" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C124" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C125" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B126" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C126" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C127" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C128" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B129" s="12" t="s">
         <v>20</v>
@@ -2413,29 +2431,29 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B130" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C130" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B131" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C131" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B132" s="4" t="s">
         <v>10</v>
@@ -2443,26 +2461,26 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B134" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C134" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B135" s="4" t="s">
         <v>10</v>
@@ -2470,202 +2488,200 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B136" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="B137" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>230</v>
-      </c>
+      <c r="A137" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C137" s="1"/>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B138" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="C138" s="12" t="s">
         <v>217</v>
-      </c>
-      <c r="C138" s="12" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B139" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C139" s="12" t="s">
         <v>217</v>
-      </c>
-      <c r="C139" s="12" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B140" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C140" s="12" t="s">
         <v>217</v>
-      </c>
-      <c r="C140" s="12" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B141" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C141" s="12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B142" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C142" s="12" t="s">
         <v>217</v>
-      </c>
-      <c r="C142" s="12" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B143" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C143" s="12" t="s">
         <v>217</v>
-      </c>
-      <c r="C143" s="12" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B144" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C144" s="12" t="s">
         <v>217</v>
-      </c>
-      <c r="C144" s="12" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B145" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C145" s="12" t="s">
         <v>217</v>
-      </c>
-      <c r="C145" s="12" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B146" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C146" s="12" t="s">
         <v>217</v>
-      </c>
-      <c r="C146" s="12" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B147" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C147" s="12" t="s">
         <v>217</v>
-      </c>
-      <c r="C147" s="12" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B148" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C148" s="12" t="s">
         <v>217</v>
-      </c>
-      <c r="C148" s="12" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B149" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C149" s="12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B150" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C150" s="12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B151" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C151" s="12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B152" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C152" s="12" t="s">
         <v>217</v>
-      </c>
-      <c r="C152" s="12" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B153" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C153" s="12" t="s">
         <v>217</v>
-      </c>
-      <c r="C153" s="12" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B154" s="4" t="s">
         <v>10</v>
@@ -2673,7 +2689,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B155" s="4" t="s">
         <v>10</v>
@@ -2681,54 +2697,54 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B156" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C156" s="12" t="s">
         <v>217</v>
-      </c>
-      <c r="C156" s="12" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B157" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C157" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B158" s="11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C158" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B159" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C159" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B160" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C160" t="s">
         <v>2</v>
@@ -2736,7 +2752,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B161" s="4" t="s">
         <v>10</v>
@@ -2744,7 +2760,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B162" s="4" t="s">
         <v>10</v>
@@ -2752,7 +2768,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B163" s="4" t="s">
         <v>10</v>
@@ -2760,7 +2776,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B164" s="4" t="s">
         <v>10</v>
@@ -2768,7 +2784,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B165" s="4" t="s">
         <v>10</v>
@@ -2776,7 +2792,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B166" s="4" t="s">
         <v>10</v>
@@ -2784,7 +2800,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B167" s="4" t="s">
         <v>10</v>
@@ -2792,7 +2808,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B168" s="4" t="s">
         <v>10</v>
@@ -2800,29 +2816,29 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B169" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C169" t="s">
         <v>214</v>
-      </c>
-      <c r="C169" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B170" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C170" t="s">
         <v>214</v>
-      </c>
-      <c r="C170" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B171" s="4" t="s">
         <v>10</v>
@@ -2830,21 +2846,21 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B172" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C172" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B173" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C173" t="s">
         <v>2</v>
@@ -2852,7 +2868,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B174" s="4" t="s">
         <v>10</v>
@@ -2860,7 +2876,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B175" s="4" t="s">
         <v>10</v>
@@ -2868,21 +2884,21 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B176" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C176" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B177" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C177" t="s">
         <v>2</v>
@@ -2890,18 +2906,18 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B178" s="11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C178" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B179" s="4" t="s">
         <v>10</v>
@@ -2909,183 +2925,183 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="11" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B180" s="11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C180" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="11" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B181" s="11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C181" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B182" s="11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C182" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B183" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C183" s="12" t="s">
         <v>217</v>
-      </c>
-      <c r="C183" s="12" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B184" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C184" s="12" t="s">
         <v>217</v>
-      </c>
-      <c r="C184" s="12" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B185" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C185" s="12" t="s">
         <v>217</v>
-      </c>
-      <c r="C185" s="12" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="12" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B186" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C186" s="12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B187" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C187" s="12" t="s">
         <v>217</v>
-      </c>
-      <c r="C187" s="12" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B188" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C188" s="12" t="s">
         <v>217</v>
-      </c>
-      <c r="C188" s="12" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B189" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C189" s="12" t="s">
         <v>217</v>
-      </c>
-      <c r="C189" s="12" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B190" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C190" s="12" t="s">
         <v>217</v>
-      </c>
-      <c r="C190" s="12" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B191" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C191" s="12" t="s">
         <v>217</v>
-      </c>
-      <c r="C191" s="12" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B192" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C192" s="12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B193" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C193" s="12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B194" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C194" s="12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B195" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C195" s="12" t="s">
         <v>217</v>
-      </c>
-      <c r="C195" s="12" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B196" s="4" t="s">
         <v>10</v>
@@ -3093,111 +3109,111 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="10" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B197" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C197" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B198" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C198" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="10" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B199" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C199" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B200" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C200" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B201" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C201" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="10" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B202" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C202" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B203" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C203" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ooSQLite - more work on the classic Rexx interface to bring it in sync with the object orientated interface.
git-svn-id: file:///local/rexx/oorexx/oorexx.svn@9310 0b6cbdbe-3aab-466e-b73a-abd511dda0a2
</commit_message>
<xml_diff>
--- a/incubator/ooSQLite/doc/StatusAllSQLiteFunctions.xlsx
+++ b/incubator/ooSQLite/doc/StatusAllSQLiteFunctions.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="243">
   <si>
     <t>sqlite3_aggregate_context</t>
   </si>
@@ -726,9 +726,6 @@
   </si>
   <si>
     <t>provided to support rare applications with unusual needs.</t>
-  </si>
-  <si>
-    <t>used whe creating new SQL functions and aggregates</t>
   </si>
   <si>
     <t>For low-level control of database files, hard to see its use in Rexx</t>
@@ -783,6 +780,12 @@
   </si>
   <si>
     <t>verb is create function</t>
+  </si>
+  <si>
+    <t>Implemented indirectly, framework passes db to UDFs</t>
+  </si>
+  <si>
+    <t>Implemented indirectly, framework uses in implementation of UDFs</t>
   </si>
 </sst>
 </file>
@@ -1244,15 +1247,15 @@
   <dimension ref="A1:C207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A107" sqref="A107"/>
+      <pane ySplit="4" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A145" sqref="A145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47" customWidth="1"/>
-    <col min="3" max="3" width="66.140625" customWidth="1"/>
+    <col min="3" max="3" width="68.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1274,14 +1277,14 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>217</v>
+      <c r="B5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1553,11 +1556,11 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>239</v>
+        <v>10</v>
       </c>
       <c r="C36" s="12"/>
     </row>
@@ -1798,14 +1801,14 @@
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="9" t="s">
+      <c r="A65" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B65" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="C65" s="12" t="s">
-        <v>231</v>
+      <c r="B65" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C65" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1833,10 +1836,10 @@
         <v>66</v>
       </c>
       <c r="B68" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C68" t="s">
         <v>239</v>
-      </c>
-      <c r="C68" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1864,10 +1867,10 @@
         <v>69</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C71" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -2052,7 +2055,7 @@
         <v>218</v>
       </c>
       <c r="C92" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -2067,11 +2070,11 @@
       <c r="A94" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C94" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -2101,7 +2104,7 @@
         <v>215</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -2134,7 +2137,7 @@
         <v>10</v>
       </c>
       <c r="C100" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -2205,7 +2208,7 @@
         <v>10</v>
       </c>
       <c r="C108" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -2243,7 +2246,7 @@
         <v>10</v>
       </c>
       <c r="C112" t="s">
-        <v>214</v>
+        <v>236</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -2254,7 +2257,7 @@
         <v>10</v>
       </c>
       <c r="C113" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -2265,7 +2268,7 @@
         <v>10</v>
       </c>
       <c r="C114" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -2276,7 +2279,7 @@
         <v>10</v>
       </c>
       <c r="C115" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -2298,7 +2301,7 @@
         <v>10</v>
       </c>
       <c r="C117" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -2320,7 +2323,7 @@
         <v>10</v>
       </c>
       <c r="C119" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -2331,7 +2334,7 @@
         <v>10</v>
       </c>
       <c r="C120" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -2475,7 +2478,7 @@
         <v>10</v>
       </c>
       <c r="C134" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -2714,7 +2717,7 @@
         <v>10</v>
       </c>
       <c r="C157" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -2736,7 +2739,7 @@
         <v>10</v>
       </c>
       <c r="C159" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -2931,7 +2934,7 @@
         <v>218</v>
       </c>
       <c r="C180" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -2942,7 +2945,7 @@
         <v>218</v>
       </c>
       <c r="C181" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -2953,18 +2956,18 @@
         <v>218</v>
       </c>
       <c r="C182" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A183" s="8" t="s">
+      <c r="A183" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="B183" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="C183" s="12" t="s">
-        <v>217</v>
+      <c r="B183" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C183" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -3148,7 +3151,7 @@
         <v>10</v>
       </c>
       <c r="C200" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
@@ -3159,7 +3162,7 @@
         <v>10</v>
       </c>
       <c r="C201" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>